<commit_message>
Added Game and Language controllers
</commit_message>
<xml_diff>
--- a/C61/Phase 1/Plannification.xlsx
+++ b/C61/Phase 1/Plannification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\CEGEP\Shift\C61\Phase 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E16EDF63-E200-42E3-8151-E824B6152806}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61CD5078-29F3-4D46-9C7E-D595B14EC619}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{BF791A61-1AC1-4C7E-B497-ABC8E6F84FF9}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="91">
   <si>
     <t>Nom</t>
   </si>
@@ -132,9 +132,6 @@
     <t>Création modèle usager</t>
   </si>
   <si>
-    <t>Création modèle word</t>
-  </si>
-  <si>
     <t>Création modèle partie</t>
   </si>
   <si>
@@ -231,9 +228,6 @@
     <t>Contrôleur word</t>
   </si>
   <si>
-    <t>Contrôleur Langage</t>
-  </si>
-  <si>
     <t>Structure HTML</t>
   </si>
   <si>
@@ -307,6 +301,12 @@
   </si>
   <si>
     <t>InGame_prep_trad.html style</t>
+  </si>
+  <si>
+    <t>Création modèle langage</t>
+  </si>
+  <si>
+    <t>addLanguage()</t>
   </si>
 </sst>
 </file>
@@ -334,12 +334,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -380,7 +386,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -410,6 +416,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -787,10 +794,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33D8B194-C08B-45A7-8AEE-FF27905754D6}">
-  <dimension ref="C3:J141"/>
+  <dimension ref="C3:K141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="I40" sqref="I40"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I49" sqref="I49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -805,12 +812,12 @@
     <col min="10" max="10" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C4" s="13" t="s">
         <v>2</v>
       </c>
@@ -825,7 +832,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:11" x14ac:dyDescent="0.25">
       <c r="F5" s="10" t="s">
         <v>18</v>
       </c>
@@ -836,7 +843,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
         <v>1</v>
       </c>
@@ -850,7 +857,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C7" s="13" t="s">
         <v>3</v>
       </c>
@@ -861,7 +868,7 @@
       </c>
       <c r="H7" s="10"/>
     </row>
-    <row r="12" spans="3:10" s="1" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:11" s="1" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="3" t="s">
         <v>12</v>
       </c>
@@ -884,13 +891,13 @@
         <v>7</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="3:10" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="3:11" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="7"/>
       <c r="D13" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="7" t="s">
@@ -909,10 +916,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="3:10" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:11" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="7"/>
       <c r="D14" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7" t="s">
@@ -931,7 +938,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C15" s="7"/>
       <c r="D15" s="2" t="s">
         <v>26</v>
@@ -952,8 +959,9 @@
       <c r="J15" s="9">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="K15" s="15"/>
+    </row>
+    <row r="16" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C16" s="3"/>
       <c r="D16" s="2"/>
       <c r="E16" s="3"/>
@@ -963,10 +971,10 @@
       <c r="I16" s="2"/>
       <c r="J16" s="9"/>
     </row>
-    <row r="17" spans="3:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C17" s="3"/>
       <c r="D17" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="2"/>
@@ -975,7 +983,7 @@
       <c r="I17" s="2"/>
       <c r="J17" s="9"/>
     </row>
-    <row r="18" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C18" s="7"/>
       <c r="D18" s="2" t="s">
         <v>21</v>
@@ -996,8 +1004,9 @@
       <c r="J18">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="K18" s="15"/>
+    </row>
+    <row r="19" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C19" s="7"/>
       <c r="D19" s="2" t="s">
         <v>22</v>
@@ -1018,8 +1027,9 @@
       <c r="J19" s="9">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="K19" s="15"/>
+    </row>
+    <row r="20" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C20" s="3"/>
       <c r="D20" s="2"/>
       <c r="E20" s="3"/>
@@ -1029,7 +1039,7 @@
       <c r="I20" s="2"/>
       <c r="J20" s="9"/>
     </row>
-    <row r="21" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="2"/>
@@ -1038,17 +1048,17 @@
       <c r="I21" s="2"/>
       <c r="J21" s="9"/>
     </row>
-    <row r="22" spans="3:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C22" s="7"/>
       <c r="D22" s="12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H22" s="6"/>
       <c r="J22">
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C23" s="7"/>
       <c r="D23" s="2" t="s">
         <v>23</v>
@@ -1070,7 +1080,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C24" s="7"/>
       <c r="D24" s="2" t="s">
         <v>24</v>
@@ -1092,7 +1102,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C25" s="7"/>
       <c r="D25" s="2" t="s">
         <v>25</v>
@@ -1114,10 +1124,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C26" s="3"/>
       <c r="D26" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E26" s="3"/>
       <c r="F26" s="2" t="s">
@@ -1133,10 +1143,10 @@
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C27" s="3"/>
       <c r="D27" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E27" s="3"/>
       <c r="F27" s="2" t="s">
@@ -1152,10 +1162,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C28" s="3"/>
       <c r="D28" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E28" s="3"/>
       <c r="F28" s="2" t="s">
@@ -1171,10 +1181,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C29" s="3"/>
       <c r="D29" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="2" t="s">
@@ -1190,7 +1200,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C30" s="3"/>
       <c r="D30" s="2"/>
       <c r="E30" s="3"/>
@@ -1199,7 +1209,7 @@
       <c r="H30" s="5"/>
       <c r="I30" s="2"/>
     </row>
-    <row r="31" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C31" s="3"/>
       <c r="D31" s="2"/>
       <c r="E31" s="3"/>
@@ -1208,7 +1218,7 @@
       <c r="H31" s="5"/>
       <c r="I31" s="2"/>
     </row>
-    <row r="32" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C32" s="3"/>
       <c r="D32" s="2"/>
       <c r="E32" s="3"/>
@@ -1217,7 +1227,7 @@
       <c r="H32" s="5"/>
       <c r="I32" s="2"/>
     </row>
-    <row r="33" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C33" s="3"/>
       <c r="D33" s="2"/>
       <c r="E33" s="3"/>
@@ -1226,10 +1236,10 @@
       <c r="H33" s="5"/>
       <c r="I33" s="2"/>
     </row>
-    <row r="34" spans="3:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C34" s="3"/>
       <c r="D34" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E34" s="3"/>
       <c r="F34" s="2"/>
@@ -1237,7 +1247,7 @@
       <c r="H34" s="5"/>
       <c r="I34" s="2"/>
     </row>
-    <row r="35" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C35" s="3"/>
       <c r="D35" s="2" t="s">
         <v>27</v>
@@ -1256,7 +1266,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C36" s="3"/>
       <c r="D36" s="2" t="s">
         <v>28</v>
@@ -1275,7 +1285,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="37" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C37" s="3"/>
       <c r="D37" s="2" t="s">
         <v>29</v>
@@ -1294,7 +1304,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="38" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C38" s="7"/>
       <c r="D38" s="2" t="s">
         <v>30</v>
@@ -1316,10 +1326,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C39" s="3"/>
       <c r="D39" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E39" s="3"/>
       <c r="F39" s="2" t="s">
@@ -1335,10 +1345,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C40" s="3"/>
       <c r="D40" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E40" s="3"/>
       <c r="F40" s="2" t="s">
@@ -1354,7 +1364,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C41" s="3"/>
       <c r="D41" s="2"/>
       <c r="E41" s="3"/>
@@ -1363,7 +1373,7 @@
       <c r="H41" s="5"/>
       <c r="I41" s="2"/>
     </row>
-    <row r="42" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C42" s="3"/>
       <c r="D42" s="2"/>
       <c r="E42" s="3"/>
@@ -1372,17 +1382,17 @@
       <c r="H42" s="5"/>
       <c r="I42" s="2"/>
     </row>
-    <row r="43" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C43" s="7"/>
       <c r="H43" s="6"/>
       <c r="J43">
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="3:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="44" spans="3:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C44" s="3"/>
       <c r="D44" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E44" s="3"/>
       <c r="F44" s="2"/>
@@ -1390,7 +1400,7 @@
       <c r="H44" s="5"/>
       <c r="I44" s="2"/>
     </row>
-    <row r="45" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C45" s="7"/>
       <c r="D45" s="2" t="s">
         <v>31</v>
@@ -1411,11 +1421,12 @@
       <c r="J45" s="9">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="K45" s="15"/>
+    </row>
+    <row r="46" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C46" s="7"/>
       <c r="D46" s="2" t="s">
-        <v>32</v>
+        <v>89</v>
       </c>
       <c r="E46" s="3"/>
       <c r="F46" s="2" t="s">
@@ -1433,11 +1444,12 @@
       <c r="J46" s="9">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="K46" s="15"/>
+    </row>
+    <row r="47" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C47" s="7"/>
       <c r="D47" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E47" s="3"/>
       <c r="F47" s="2" t="s">
@@ -1455,11 +1467,12 @@
       <c r="J47" s="9">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="K47" s="15"/>
+    </row>
+    <row r="48" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C48" s="7"/>
       <c r="D48" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E48" s="3"/>
       <c r="F48" s="2" t="s">
@@ -1475,11 +1488,12 @@
         <v>14</v>
       </c>
       <c r="J48" s="9"/>
-    </row>
-    <row r="49" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="K48" s="15"/>
+    </row>
+    <row r="49" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C49" s="7"/>
       <c r="D49" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E49" s="3"/>
       <c r="F49" s="2" t="s">
@@ -1497,11 +1511,12 @@
       <c r="J49">
         <v>5</v>
       </c>
-    </row>
-    <row r="50" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="K49" s="15"/>
+    </row>
+    <row r="50" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C50" s="7"/>
       <c r="D50" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E50" s="3"/>
       <c r="F50" s="2" t="s">
@@ -1517,7 +1532,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="51" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C51" s="3"/>
       <c r="D51" s="2"/>
       <c r="E51" s="3"/>
@@ -1526,10 +1541,10 @@
       <c r="H51" s="5"/>
       <c r="I51" s="2"/>
     </row>
-    <row r="52" spans="3:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="52" spans="3:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C52" s="3"/>
       <c r="D52" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E52" s="3"/>
       <c r="F52" s="2"/>
@@ -1537,10 +1552,10 @@
       <c r="H52" s="5"/>
       <c r="I52" s="2"/>
     </row>
-    <row r="53" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C53" s="7"/>
       <c r="D53" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E53" s="3"/>
       <c r="F53" s="2" t="s">
@@ -1559,10 +1574,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C54" s="7"/>
       <c r="D54" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E54" s="3"/>
       <c r="F54" s="2" t="s">
@@ -1581,10 +1596,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C55" s="7"/>
       <c r="D55" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E55" s="3"/>
       <c r="F55" s="2" t="s">
@@ -1603,10 +1618,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C56" s="7"/>
       <c r="D56" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E56" s="3"/>
       <c r="F56" s="2" t="s">
@@ -1625,10 +1640,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C57" s="7"/>
       <c r="D57" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E57" s="3"/>
       <c r="F57" s="2" t="s">
@@ -1646,8 +1661,9 @@
       <c r="J57">
         <v>5</v>
       </c>
-    </row>
-    <row r="58" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="K57" s="15"/>
+    </row>
+    <row r="58" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C58" s="3"/>
       <c r="D58" s="2"/>
       <c r="E58" s="3"/>
@@ -1656,10 +1672,10 @@
       <c r="H58" s="5"/>
       <c r="I58" s="2"/>
     </row>
-    <row r="59" spans="3:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="59" spans="3:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C59" s="3"/>
       <c r="D59" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E59" s="3"/>
       <c r="F59" s="2"/>
@@ -1667,10 +1683,10 @@
       <c r="H59" s="5"/>
       <c r="I59" s="2"/>
     </row>
-    <row r="60" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C60" s="7"/>
       <c r="D60" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E60" s="3"/>
       <c r="F60" s="2" t="s">
@@ -1689,10 +1705,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C61" s="7"/>
       <c r="D61" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E61" s="3"/>
       <c r="F61" s="2" t="s">
@@ -1711,10 +1727,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C62" s="7"/>
       <c r="D62" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E62" s="3"/>
       <c r="F62" s="2" t="s">
@@ -1733,7 +1749,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C63" s="3"/>
       <c r="D63" s="2"/>
       <c r="E63" s="3"/>
@@ -1742,10 +1758,10 @@
       <c r="H63" s="5"/>
       <c r="I63" s="2"/>
     </row>
-    <row r="64" spans="3:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="64" spans="3:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C64" s="3"/>
       <c r="D64" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E64" s="3"/>
       <c r="F64" s="2"/>
@@ -1756,7 +1772,7 @@
     <row r="65" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C65" s="7"/>
       <c r="D65" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E65" s="3"/>
       <c r="F65" s="2" t="s">
@@ -1778,7 +1794,7 @@
     <row r="66" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C66" s="7"/>
       <c r="D66" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E66" s="3"/>
       <c r="F66" s="2" t="s">
@@ -1800,7 +1816,7 @@
     <row r="67" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C67" s="7"/>
       <c r="D67" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E67" s="3"/>
       <c r="F67" s="2" t="s">
@@ -1821,18 +1837,26 @@
     </row>
     <row r="68" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C68" s="3"/>
-      <c r="D68" s="2"/>
+      <c r="D68" s="2" t="s">
+        <v>90</v>
+      </c>
       <c r="E68" s="3"/>
-      <c r="F68" s="2"/>
-      <c r="G68" s="2"/>
-      <c r="H68" s="5"/>
-      <c r="I68" s="2"/>
-    </row>
-    <row r="69" spans="3:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F68" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G68" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H68" s="5">
+        <v>35</v>
+      </c>
+      <c r="I68" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="69" spans="3:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C69" s="3"/>
-      <c r="D69" s="12" t="s">
-        <v>65</v>
-      </c>
+      <c r="D69" s="12"/>
       <c r="E69" s="3"/>
       <c r="F69" s="2"/>
       <c r="G69" s="2"/>
@@ -1841,24 +1865,10 @@
     </row>
     <row r="70" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C70" s="3"/>
-      <c r="D70" s="2" t="s">
-        <v>50</v>
-      </c>
       <c r="E70" s="3"/>
-      <c r="F70" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G70" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H70" s="5">
-        <v>35</v>
-      </c>
-      <c r="I70" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="71" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="H70" s="6"/>
+    </row>
+    <row r="71" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C71" s="3"/>
       <c r="D71" s="2"/>
       <c r="E71" s="3"/>
@@ -1867,10 +1877,10 @@
       <c r="H71" s="5"/>
       <c r="I71" s="2"/>
     </row>
-    <row r="72" spans="3:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="72" spans="3:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C72" s="3"/>
       <c r="D72" s="12" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E72" s="3"/>
       <c r="F72" s="2"/>
@@ -1881,7 +1891,7 @@
     <row r="73" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C73" s="3"/>
       <c r="D73" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E73" s="3"/>
       <c r="F73" s="2" t="s">
@@ -1897,7 +1907,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="74" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C74" s="3"/>
       <c r="D74" s="2"/>
       <c r="E74" s="3"/>
@@ -1906,10 +1916,10 @@
       <c r="H74" s="5"/>
       <c r="I74" s="2"/>
     </row>
-    <row r="75" spans="3:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="75" spans="3:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C75" s="3"/>
       <c r="D75" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E75" s="3"/>
       <c r="F75" s="2"/>
@@ -1920,7 +1930,7 @@
     <row r="76" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C76" s="7"/>
       <c r="D76" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E76" s="3"/>
       <c r="F76" s="2" t="s">
@@ -1939,7 +1949,7 @@
     <row r="77" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C77" s="7"/>
       <c r="D77" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E77" s="3"/>
       <c r="F77" s="2" t="s">
@@ -1967,7 +1977,7 @@
     <row r="79" spans="3:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C79" s="3"/>
       <c r="D79" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E79" s="3"/>
       <c r="F79" s="2"/>
@@ -1978,7 +1988,7 @@
     <row r="80" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C80" s="7"/>
       <c r="D80" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E80" s="3"/>
       <c r="F80" s="2" t="s">
@@ -2000,7 +2010,7 @@
     <row r="81" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C81" s="7"/>
       <c r="D81" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E81" s="3"/>
       <c r="F81" s="2" t="s">
@@ -2022,7 +2032,7 @@
     <row r="82" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C82" s="7"/>
       <c r="D82" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E82" s="3"/>
       <c r="F82" s="2" t="s">
@@ -2041,10 +2051,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C83" s="7"/>
       <c r="D83" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E83" s="3"/>
       <c r="F83" s="2" t="s">
@@ -2066,7 +2076,7 @@
     <row r="84" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C84" s="7"/>
       <c r="D84" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E84" s="3"/>
       <c r="F84" s="2" t="s">
@@ -2085,10 +2095,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C85" s="7"/>
       <c r="D85" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E85" s="3"/>
       <c r="F85" s="2" t="s">
@@ -2110,7 +2120,7 @@
     <row r="86" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C86" s="7"/>
       <c r="D86" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E86" s="3"/>
       <c r="F86" s="2" t="s">
@@ -2129,7 +2139,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C87" s="3"/>
       <c r="D87" s="2"/>
       <c r="E87" s="3"/>
@@ -2139,10 +2149,10 @@
       <c r="I87" s="2"/>
       <c r="J87" s="9"/>
     </row>
-    <row r="88" spans="3:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="88" spans="3:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C88" s="3"/>
       <c r="D88" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E88" s="3"/>
       <c r="F88" s="2"/>
@@ -2151,10 +2161,10 @@
       <c r="I88" s="2"/>
       <c r="J88" s="9"/>
     </row>
-    <row r="89" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C89" s="7"/>
       <c r="D89" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E89" s="3"/>
       <c r="F89" s="2" t="s">
@@ -2176,7 +2186,7 @@
     <row r="90" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C90" s="7"/>
       <c r="D90" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E90" s="3"/>
       <c r="F90" s="2" t="s">
@@ -2195,10 +2205,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C91" s="7"/>
       <c r="D91" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E91" s="3"/>
       <c r="F91" s="2" t="s">
@@ -2229,7 +2239,7 @@
     <row r="93" spans="3:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C93" s="3"/>
       <c r="D93" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E93" s="3"/>
       <c r="F93" s="2"/>
@@ -2240,7 +2250,7 @@
     <row r="94" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C94" s="7"/>
       <c r="D94" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E94" s="3"/>
       <c r="F94" s="2" t="s">
@@ -2259,10 +2269,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="95" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C95" s="7"/>
       <c r="D95" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E95" s="3"/>
       <c r="F95" s="2" t="s">
@@ -2284,7 +2294,7 @@
     <row r="96" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C96" s="7"/>
       <c r="D96" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E96" s="3"/>
       <c r="F96" s="2" t="s">
@@ -2303,10 +2313,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="97" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C97" s="7"/>
       <c r="D97" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E97" s="3"/>
       <c r="F97" s="2" t="s">
@@ -2328,7 +2338,7 @@
     <row r="98" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C98" s="7"/>
       <c r="D98" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E98" s="3"/>
       <c r="F98" s="2" t="s">
@@ -2347,10 +2357,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="99" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C99" s="7"/>
       <c r="D99" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F99" t="s">
         <v>17</v>
@@ -2372,7 +2382,7 @@
     <row r="101" spans="3:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C101" s="3"/>
       <c r="D101" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E101" s="3"/>
       <c r="F101" s="2"/>
@@ -2383,7 +2393,7 @@
     <row r="102" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C102" s="7"/>
       <c r="D102" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E102" s="3"/>
       <c r="F102" s="2" t="s">
@@ -2399,10 +2409,10 @@
         <v>16</v>
       </c>
     </row>
-    <row r="103" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C103" s="7"/>
       <c r="D103" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F103" t="s">
         <v>18</v>
@@ -2537,13 +2547,13 @@
     <mergeCell ref="C4:D4"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G15:G21 G44:G188 G23:G42" xr:uid="{737FDF90-EFB8-4011-8F39-3F216A04A4E8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G15:G21 G23:G42 G71:G188 G44:G69" xr:uid="{737FDF90-EFB8-4011-8F39-3F216A04A4E8}">
       <formula1>$G$4:$G$7</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I13:I21 I44:I141 I23:I42" xr:uid="{D545C4CF-8505-4E3A-8974-2AE18E2A1E4D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I13:I21 I23:I42 I71:I141 I44:I69" xr:uid="{D545C4CF-8505-4E3A-8974-2AE18E2A1E4D}">
       <formula1>$H$4:$H$6</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F13:F21 F44:F141 F23:F42" xr:uid="{0789BEBC-1BFC-4915-ADA0-26973175C7BB}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F13:F21 F23:F42 F71:F141 F44:F69" xr:uid="{0789BEBC-1BFC-4915-ADA0-26973175C7BB}">
       <formula1>$F$4:$F$6</formula1>
     </dataValidation>
   </dataValidations>
@@ -2573,16 +2583,16 @@
   <sheetData>
     <row r="6" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" t="s">
         <v>35</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>36</v>
-      </c>
-      <c r="G6" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="7" spans="4:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2641,7 +2651,7 @@
     </row>
     <row r="11" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E11">
         <f>SUM(E7:E10)</f>

</xml_diff>

<commit_message>
Added base navbar on index page. Missing a lot of style
</commit_message>
<xml_diff>
--- a/C61/Phase 1/Plannification.xlsx
+++ b/C61/Phase 1/Plannification.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\CEGEP\Shift\C61\Phase 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61CD5078-29F3-4D46-9C7E-D595B14EC619}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DAF098D-8000-419E-BA31-4C508C19F53C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{BF791A61-1AC1-4C7E-B497-ABC8E6F84FF9}"/>
+    <workbookView minimized="1" xWindow="8085" yWindow="4005" windowWidth="12150" windowHeight="11835" xr2:uid="{BF791A61-1AC1-4C7E-B497-ABC8E6F84FF9}"/>
   </bookViews>
   <sheets>
     <sheet name="Plannification" sheetId="1" r:id="rId1"/>
@@ -414,9 +414,9 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -796,8 +796,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33D8B194-C08B-45A7-8AEE-FF27905754D6}">
   <dimension ref="C3:K141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I49" sqref="I49"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -818,10 +818,10 @@
       </c>
     </row>
     <row r="4" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="14"/>
+      <c r="D4" s="15"/>
       <c r="F4" s="10" t="s">
         <v>17</v>
       </c>
@@ -858,10 +858,10 @@
       </c>
     </row>
     <row r="7" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="14"/>
+      <c r="D7" s="15"/>
       <c r="F7" s="10"/>
       <c r="G7" s="10" t="s">
         <v>11</v>
@@ -959,7 +959,7 @@
       <c r="J15" s="9">
         <v>1</v>
       </c>
-      <c r="K15" s="15"/>
+      <c r="K15" s="13"/>
     </row>
     <row r="16" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C16" s="3"/>
@@ -1004,7 +1004,7 @@
       <c r="J18">
         <v>5</v>
       </c>
-      <c r="K18" s="15"/>
+      <c r="K18" s="13"/>
     </row>
     <row r="19" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C19" s="7"/>
@@ -1027,7 +1027,7 @@
       <c r="J19" s="9">
         <v>1</v>
       </c>
-      <c r="K19" s="15"/>
+      <c r="K19" s="13"/>
     </row>
     <row r="20" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C20" s="3"/>
@@ -1301,7 +1301,7 @@
         <v>120</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="38" spans="3:11" x14ac:dyDescent="0.25">
@@ -1421,7 +1421,7 @@
       <c r="J45" s="9">
         <v>1</v>
       </c>
-      <c r="K45" s="15"/>
+      <c r="K45" s="13"/>
     </row>
     <row r="46" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C46" s="7"/>
@@ -1444,7 +1444,7 @@
       <c r="J46" s="9">
         <v>1</v>
       </c>
-      <c r="K46" s="15"/>
+      <c r="K46" s="13"/>
     </row>
     <row r="47" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C47" s="7"/>
@@ -1467,7 +1467,7 @@
       <c r="J47" s="9">
         <v>1</v>
       </c>
-      <c r="K47" s="15"/>
+      <c r="K47" s="13"/>
     </row>
     <row r="48" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C48" s="7"/>
@@ -1488,7 +1488,7 @@
         <v>14</v>
       </c>
       <c r="J48" s="9"/>
-      <c r="K48" s="15"/>
+      <c r="K48" s="13"/>
     </row>
     <row r="49" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C49" s="7"/>
@@ -1511,7 +1511,7 @@
       <c r="J49">
         <v>5</v>
       </c>
-      <c r="K49" s="15"/>
+      <c r="K49" s="13"/>
     </row>
     <row r="50" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C50" s="7"/>
@@ -1661,7 +1661,7 @@
       <c r="J57">
         <v>5</v>
       </c>
-      <c r="K57" s="15"/>
+      <c r="K57" s="13"/>
     </row>
     <row r="58" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C58" s="3"/>
@@ -2601,15 +2601,15 @@
       </c>
       <c r="E7" s="8">
         <f>COUNTIF(Plannification!I13:I141,Plannification!H4)</f>
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F7" s="11">
         <f>(COUNTIFS(Plannification!G:G,"Facile",Plannification!I:I,"Sprint 1")*1+COUNTIFS(Plannification!G:G,"Moyen",Plannification!I:I,"Sprint 1")*5+COUNTIFS(Plannification!G:G,"Difficile",Plannification!I:I,"Sprint 1")*10+COUNTIFS(Plannification!G:G,"Incertain",Plannification!I:I,"Sprint 1")*7.5)/COUNTA(Plannification!G13:G102)</f>
-        <v>1.9732142857142858</v>
+        <v>1.7946428571428572</v>
       </c>
       <c r="G7">
         <f>SUMIF(Plannification!I13:I140,Plannification!H4,Plannification!H13:H140)</f>
-        <v>1380</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="8" spans="4:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2635,15 +2635,15 @@
       </c>
       <c r="E9">
         <f>COUNTIF(Plannification!I13:I141,Plannification!H6)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F9" s="11">
         <f>(COUNTIFS(Plannification!G:G,"Facile",Plannification!I:I,"Sprint 3")*1+COUNTIFS(Plannification!G:G,"Moyen",Plannification!I:I,"Sprint 3")*5+COUNTIFS(Plannification!G:G,"Difficile",Plannification!I:I,"Sprint 3")*10+COUNTIFS(Plannification!G:G,"Incertain",Plannification!I:I,"Sprint 3")*7.5)/COUNTA(Plannification!G13:G102)</f>
-        <v>1.0625</v>
+        <v>1.2410714285714286</v>
       </c>
       <c r="G9">
         <f>SUMIF(Plannification!I13:I140,Plannification!H6,Plannification!H13:H140)</f>
-        <v>720</v>
+        <v>840</v>
       </c>
     </row>
     <row r="10" spans="4:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Tweaked word position for better center in factory.js
</commit_message>
<xml_diff>
--- a/C61/Phase 1/Plannification.xlsx
+++ b/C61/Phase 1/Plannification.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\CEGEP\Shift\C61\Phase 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DAF098D-8000-419E-BA31-4C508C19F53C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBBE38D8-9BDF-4538-B408-FC3C84885C8A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="8085" yWindow="4005" windowWidth="12150" windowHeight="11835" xr2:uid="{BF791A61-1AC1-4C7E-B497-ABC8E6F84FF9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{BF791A61-1AC1-4C7E-B497-ABC8E6F84FF9}"/>
   </bookViews>
   <sheets>
     <sheet name="Plannification" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="102">
   <si>
     <t>Nom</t>
   </si>
@@ -307,6 +307,39 @@
   </si>
   <si>
     <t>addLanguage()</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>Explication</t>
+  </si>
+  <si>
+    <t>Pour le moment, j'ai uniquement 1 language disponible. L'important est que je puisses montrer que ça fonctionne, mais le reste du projet est plus important. Il est toujours possible de rajouter par la suite.</t>
+  </si>
+  <si>
+    <t>Difficulté à bien centrer dans un canvas et page fait vide</t>
+  </si>
+  <si>
+    <t>Pas une priorité. Repoussé au sprint 3 si le temps me le permet</t>
+  </si>
+  <si>
+    <t>Fonction inutile</t>
+  </si>
+  <si>
+    <t>getNoun()</t>
+  </si>
+  <si>
+    <t>getExpression()</t>
+  </si>
+  <si>
+    <t>calcPX</t>
+  </si>
+  <si>
+    <t>Il manque le footer - Le style de cette page a pris beaucoup plus de temps que prévu</t>
+  </si>
+  <si>
+    <t>Manque quelques images</t>
   </si>
 </sst>
 </file>
@@ -386,7 +419,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -414,14 +447,36 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="8">
+    <dxf>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
@@ -468,17 +523,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6A6624AC-1B89-41F0-97C8-B731967F0432}" name="Table2" displayName="Table2" ref="C12:J141" totalsRowShown="0" headerRowDxfId="5" tableBorderDxfId="4">
-  <autoFilter ref="C12:J141" xr:uid="{45C19323-F7FF-4676-9643-D7E43592846B}"/>
-  <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{BEB73C37-012B-4855-AD2E-BF3FC3282F6F}" name="No tâche" dataDxfId="3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6A6624AC-1B89-41F0-97C8-B731967F0432}" name="Table2" displayName="Table2" ref="C12:L147" totalsRowShown="0" headerRowDxfId="7" tableBorderDxfId="6">
+  <autoFilter ref="C12:L147" xr:uid="{45C19323-F7FF-4676-9643-D7E43592846B}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{BEB73C37-012B-4855-AD2E-BF3FC3282F6F}" name="No tâche" dataDxfId="5"/>
     <tableColumn id="5" xr3:uid="{9FB5B8D6-EB0F-453F-9F7B-590278B05C91}" name="Titre"/>
-    <tableColumn id="6" xr3:uid="{1E70752F-88D9-4030-A938-450361DD5532}" name="Tâches préalables" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{1E70752F-88D9-4030-A938-450361DD5532}" name="Tâches préalables" dataDxfId="4"/>
     <tableColumn id="7" xr3:uid="{F97670F9-2262-48ED-AA08-62F6F9DE6530}" name="Priorité"/>
     <tableColumn id="8" xr3:uid="{BC349C26-3803-4636-8F9B-94A4C9F5CD7E}" name="Difficulté"/>
-    <tableColumn id="9" xr3:uid="{4BB0A79B-2A72-4D99-BAAE-1417C9CAB8ED}" name="Estimation du temps (Minutes)" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{4BB0A79B-2A72-4D99-BAAE-1417C9CAB8ED}" name="Estimation du temps (Minutes)" dataDxfId="3"/>
     <tableColumn id="10" xr3:uid="{1E1E24DC-14B2-493C-89A6-C8A50BD4426E}" name="No Sprint"/>
     <tableColumn id="2" xr3:uid="{A39DC1DB-5846-4641-8706-F0F11BD2DE3F}" name="Colonne1"/>
+    <tableColumn id="3" xr3:uid="{C66CE7BF-5C52-44E8-8EF8-E28096D37B9A}" name="%" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{70C6D8C4-FE57-4C67-9C5A-4753AD78373B}" name="Explication" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -490,7 +547,7 @@
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{7129546F-9161-4E67-83CD-24985F439177}" name="Sprint"/>
     <tableColumn id="3" xr3:uid="{EE02ED3A-9EB9-4163-82D8-E449A890A7D2}" name="Nombre de tâche"/>
-    <tableColumn id="4" xr3:uid="{7A15D220-8097-4D1D-9F42-CA005B326E2A}" name="Difficulté moyenne" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{7A15D220-8097-4D1D-9F42-CA005B326E2A}" name="Difficulté moyenne" dataDxfId="2"/>
     <tableColumn id="5" xr3:uid="{20438E1E-C106-4680-8557-D00CA50BC5A6}" name="Temps total requis"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -794,10 +851,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33D8B194-C08B-45A7-8AEE-FF27905754D6}">
-  <dimension ref="C3:K141"/>
+  <dimension ref="C3:L147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="I37" sqref="I37"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -810,18 +867,20 @@
     <col min="8" max="8" width="14.7109375" customWidth="1"/>
     <col min="9" max="9" width="14.85546875" customWidth="1"/>
     <col min="10" max="10" width="0" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="11.140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="37.85546875" style="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C4" s="14" t="s">
+    <row r="4" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C4" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="15"/>
+      <c r="D4" s="14"/>
       <c r="F4" s="10" t="s">
         <v>17</v>
       </c>
@@ -832,7 +891,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:12" x14ac:dyDescent="0.25">
       <c r="F5" s="10" t="s">
         <v>18</v>
       </c>
@@ -843,7 +902,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
         <v>1</v>
       </c>
@@ -857,18 +916,18 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C7" s="14" t="s">
+    <row r="7" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C7" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="15"/>
+      <c r="D7" s="14"/>
       <c r="F7" s="10"/>
       <c r="G7" s="10" t="s">
         <v>11</v>
       </c>
       <c r="H7" s="10"/>
     </row>
-    <row r="12" spans="3:11" s="1" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:12" s="1" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="3" t="s">
         <v>12</v>
       </c>
@@ -893,8 +952,14 @@
       <c r="J12" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="13" spans="3:11" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K12" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="L12" s="20" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="3:12" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="7"/>
       <c r="D13" s="7" t="s">
         <v>37</v>
@@ -915,8 +980,12 @@
       <c r="J13" s="9">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="3:11" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K13" s="17">
+        <v>1</v>
+      </c>
+      <c r="L13" s="21"/>
+    </row>
+    <row r="14" spans="3:12" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="7"/>
       <c r="D14" s="7" t="s">
         <v>33</v>
@@ -937,8 +1006,14 @@
       <c r="J14" s="9">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="K14" s="17">
+        <v>0.75</v>
+      </c>
+      <c r="L14" s="21" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="15" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C15" s="7"/>
       <c r="D15" s="2" t="s">
         <v>26</v>
@@ -959,9 +1034,11 @@
       <c r="J15" s="9">
         <v>1</v>
       </c>
-      <c r="K15" s="13"/>
-    </row>
-    <row r="16" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="K15" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C16" s="3"/>
       <c r="D16" s="2"/>
       <c r="E16" s="3"/>
@@ -971,7 +1048,7 @@
       <c r="I16" s="2"/>
       <c r="J16" s="9"/>
     </row>
-    <row r="17" spans="3:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C17" s="3"/>
       <c r="D17" s="12" t="s">
         <v>61</v>
@@ -983,7 +1060,7 @@
       <c r="I17" s="2"/>
       <c r="J17" s="9"/>
     </row>
-    <row r="18" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C18" s="7"/>
       <c r="D18" s="2" t="s">
         <v>21</v>
@@ -1004,9 +1081,11 @@
       <c r="J18">
         <v>5</v>
       </c>
-      <c r="K18" s="13"/>
-    </row>
-    <row r="19" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="K18" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="3:12" ht="90" x14ac:dyDescent="0.25">
       <c r="C19" s="7"/>
       <c r="D19" s="2" t="s">
         <v>22</v>
@@ -1027,9 +1106,14 @@
       <c r="J19" s="9">
         <v>1</v>
       </c>
-      <c r="K19" s="13"/>
-    </row>
-    <row r="20" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="K19" s="18">
+        <v>0.33</v>
+      </c>
+      <c r="L19" s="19" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="20" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C20" s="3"/>
       <c r="D20" s="2"/>
       <c r="E20" s="3"/>
@@ -1039,7 +1123,7 @@
       <c r="I20" s="2"/>
       <c r="J20" s="9"/>
     </row>
-    <row r="21" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="2"/>
@@ -1048,7 +1132,7 @@
       <c r="I21" s="2"/>
       <c r="J21" s="9"/>
     </row>
-    <row r="22" spans="3:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C22" s="7"/>
       <c r="D22" s="12" t="s">
         <v>64</v>
@@ -1058,7 +1142,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C23" s="7"/>
       <c r="D23" s="2" t="s">
         <v>23</v>
@@ -1079,8 +1163,11 @@
       <c r="J23">
         <v>5</v>
       </c>
-    </row>
-    <row r="24" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="K23" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C24" s="7"/>
       <c r="D24" s="2" t="s">
         <v>24</v>
@@ -1101,8 +1188,11 @@
       <c r="J24">
         <v>5</v>
       </c>
-    </row>
-    <row r="25" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="K24" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C25" s="7"/>
       <c r="D25" s="2" t="s">
         <v>25</v>
@@ -1124,7 +1214,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C26" s="3"/>
       <c r="D26" s="2" t="s">
         <v>83</v>
@@ -1142,8 +1232,11 @@
       <c r="I26" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="27" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="K26" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C27" s="3"/>
       <c r="D27" s="2" t="s">
         <v>84</v>
@@ -1161,8 +1254,11 @@
       <c r="I27" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="28" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="K27" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C28" s="3"/>
       <c r="D28" s="2" t="s">
         <v>85</v>
@@ -1180,8 +1276,11 @@
       <c r="I28" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="29" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="K28" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C29" s="3"/>
       <c r="D29" s="2" t="s">
         <v>86</v>
@@ -1199,8 +1298,11 @@
       <c r="I29" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="30" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="K29" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C30" s="3"/>
       <c r="D30" s="2"/>
       <c r="E30" s="3"/>
@@ -1209,7 +1311,7 @@
       <c r="H30" s="5"/>
       <c r="I30" s="2"/>
     </row>
-    <row r="31" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C31" s="3"/>
       <c r="D31" s="2"/>
       <c r="E31" s="3"/>
@@ -1218,7 +1320,7 @@
       <c r="H31" s="5"/>
       <c r="I31" s="2"/>
     </row>
-    <row r="32" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C32" s="3"/>
       <c r="D32" s="2"/>
       <c r="E32" s="3"/>
@@ -1227,7 +1329,7 @@
       <c r="H32" s="5"/>
       <c r="I32" s="2"/>
     </row>
-    <row r="33" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C33" s="3"/>
       <c r="D33" s="2"/>
       <c r="E33" s="3"/>
@@ -1236,7 +1338,7 @@
       <c r="H33" s="5"/>
       <c r="I33" s="2"/>
     </row>
-    <row r="34" spans="3:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C34" s="3"/>
       <c r="D34" s="12" t="s">
         <v>60</v>
@@ -1247,7 +1349,7 @@
       <c r="H34" s="5"/>
       <c r="I34" s="2"/>
     </row>
-    <row r="35" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:12" ht="45" x14ac:dyDescent="0.25">
       <c r="C35" s="3"/>
       <c r="D35" s="2" t="s">
         <v>27</v>
@@ -1265,8 +1367,14 @@
       <c r="I35" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="36" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="K35" s="15">
+        <v>0.85</v>
+      </c>
+      <c r="L35" s="19" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="3:12" ht="30" x14ac:dyDescent="0.25">
       <c r="C36" s="3"/>
       <c r="D36" s="2" t="s">
         <v>28</v>
@@ -1284,8 +1392,14 @@
       <c r="I36" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="37" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="K36" s="15">
+        <v>0.85</v>
+      </c>
+      <c r="L36" s="19" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="37" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C37" s="3"/>
       <c r="D37" s="2" t="s">
         <v>29</v>
@@ -1304,7 +1418,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C38" s="7"/>
       <c r="D38" s="2" t="s">
         <v>30</v>
@@ -1325,8 +1439,11 @@
       <c r="J38">
         <v>5</v>
       </c>
-    </row>
-    <row r="39" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="K38" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C39" s="3"/>
       <c r="D39" s="2" t="s">
         <v>87</v>
@@ -1345,7 +1462,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C40" s="3"/>
       <c r="D40" s="2" t="s">
         <v>88</v>
@@ -1363,8 +1480,11 @@
       <c r="I40" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="41" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="K40" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C41" s="3"/>
       <c r="D41" s="2"/>
       <c r="E41" s="3"/>
@@ -1373,7 +1493,7 @@
       <c r="H41" s="5"/>
       <c r="I41" s="2"/>
     </row>
-    <row r="42" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C42" s="3"/>
       <c r="D42" s="2"/>
       <c r="E42" s="3"/>
@@ -1382,14 +1502,14 @@
       <c r="H42" s="5"/>
       <c r="I42" s="2"/>
     </row>
-    <row r="43" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C43" s="7"/>
       <c r="H43" s="6"/>
       <c r="J43">
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="3:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="3:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C44" s="3"/>
       <c r="D44" s="12" t="s">
         <v>57</v>
@@ -1400,7 +1520,7 @@
       <c r="H44" s="5"/>
       <c r="I44" s="2"/>
     </row>
-    <row r="45" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C45" s="7"/>
       <c r="D45" s="2" t="s">
         <v>31</v>
@@ -1421,9 +1541,11 @@
       <c r="J45" s="9">
         <v>1</v>
       </c>
-      <c r="K45" s="13"/>
-    </row>
-    <row r="46" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="K45" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C46" s="7"/>
       <c r="D46" s="2" t="s">
         <v>89</v>
@@ -1444,9 +1566,11 @@
       <c r="J46" s="9">
         <v>1</v>
       </c>
-      <c r="K46" s="13"/>
-    </row>
-    <row r="47" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="K46" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C47" s="7"/>
       <c r="D47" s="2" t="s">
         <v>32</v>
@@ -1467,9 +1591,11 @@
       <c r="J47" s="9">
         <v>1</v>
       </c>
-      <c r="K47" s="13"/>
-    </row>
-    <row r="48" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="K47" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C48" s="7"/>
       <c r="D48" s="2" t="s">
         <v>46</v>
@@ -1488,9 +1614,11 @@
         <v>14</v>
       </c>
       <c r="J48" s="9"/>
-      <c r="K48" s="13"/>
-    </row>
-    <row r="49" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="K48" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C49" s="7"/>
       <c r="D49" s="2" t="s">
         <v>38</v>
@@ -1511,9 +1639,11 @@
       <c r="J49">
         <v>5</v>
       </c>
-      <c r="K49" s="13"/>
-    </row>
-    <row r="50" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="K49" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C50" s="7"/>
       <c r="D50" s="2" t="s">
         <v>45</v>
@@ -1532,7 +1662,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="51" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C51" s="3"/>
       <c r="D51" s="2"/>
       <c r="E51" s="3"/>
@@ -1541,7 +1671,7 @@
       <c r="H51" s="5"/>
       <c r="I51" s="2"/>
     </row>
-    <row r="52" spans="3:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="3:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C52" s="3"/>
       <c r="D52" s="12" t="s">
         <v>58</v>
@@ -1552,7 +1682,7 @@
       <c r="H52" s="5"/>
       <c r="I52" s="2"/>
     </row>
-    <row r="53" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C53" s="7"/>
       <c r="D53" s="2" t="s">
         <v>48</v>
@@ -1573,8 +1703,11 @@
       <c r="J53">
         <v>5</v>
       </c>
-    </row>
-    <row r="54" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="K53" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C54" s="7"/>
       <c r="D54" s="2" t="s">
         <v>62</v>
@@ -1595,8 +1728,11 @@
       <c r="J54">
         <v>5</v>
       </c>
-    </row>
-    <row r="55" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="K54" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C55" s="7"/>
       <c r="D55" s="2" t="s">
         <v>49</v>
@@ -1618,7 +1754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C56" s="7"/>
       <c r="D56" s="2" t="s">
         <v>50</v>
@@ -1640,7 +1776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C57" s="7"/>
       <c r="D57" s="2" t="s">
         <v>51</v>
@@ -1661,9 +1797,9 @@
       <c r="J57">
         <v>5</v>
       </c>
-      <c r="K57" s="13"/>
-    </row>
-    <row r="58" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="K57" s="18"/>
+    </row>
+    <row r="58" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C58" s="3"/>
       <c r="D58" s="2"/>
       <c r="E58" s="3"/>
@@ -1672,7 +1808,7 @@
       <c r="H58" s="5"/>
       <c r="I58" s="2"/>
     </row>
-    <row r="59" spans="3:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="3:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C59" s="3"/>
       <c r="D59" s="12" t="s">
         <v>59</v>
@@ -1683,7 +1819,7 @@
       <c r="H59" s="5"/>
       <c r="I59" s="2"/>
     </row>
-    <row r="60" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C60" s="7"/>
       <c r="D60" s="2" t="s">
         <v>49</v>
@@ -1704,8 +1840,11 @@
       <c r="J60" s="9">
         <v>1</v>
       </c>
-    </row>
-    <row r="61" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="K60" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="3:12" ht="30" x14ac:dyDescent="0.25">
       <c r="C61" s="7"/>
       <c r="D61" s="2" t="s">
         <v>62</v>
@@ -1726,8 +1865,14 @@
       <c r="J61">
         <v>5</v>
       </c>
-    </row>
-    <row r="62" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="K61" s="15">
+        <v>0</v>
+      </c>
+      <c r="L61" s="19" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="62" spans="3:12" ht="30" x14ac:dyDescent="0.25">
       <c r="C62" s="7"/>
       <c r="D62" s="2" t="s">
         <v>48</v>
@@ -1748,8 +1893,14 @@
       <c r="J62">
         <v>5</v>
       </c>
-    </row>
-    <row r="63" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="K62" s="15">
+        <v>0</v>
+      </c>
+      <c r="L62" s="19" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="63" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C63" s="3"/>
       <c r="D63" s="2"/>
       <c r="E63" s="3"/>
@@ -1758,7 +1909,7 @@
       <c r="H63" s="5"/>
       <c r="I63" s="2"/>
     </row>
-    <row r="64" spans="3:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="3:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C64" s="3"/>
       <c r="D64" s="12" t="s">
         <v>63</v>
@@ -1769,7 +1920,7 @@
       <c r="H64" s="5"/>
       <c r="I64" s="2"/>
     </row>
-    <row r="65" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C65" s="7"/>
       <c r="D65" s="2" t="s">
         <v>49</v>
@@ -1790,8 +1941,11 @@
       <c r="J65">
         <v>7.5</v>
       </c>
-    </row>
-    <row r="66" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="K65" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="3:12" ht="30" x14ac:dyDescent="0.25">
       <c r="C66" s="7"/>
       <c r="D66" s="2" t="s">
         <v>62</v>
@@ -1812,8 +1966,14 @@
       <c r="J66">
         <v>5</v>
       </c>
-    </row>
-    <row r="67" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="K66" s="15">
+        <v>0</v>
+      </c>
+      <c r="L66" s="19" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="67" spans="3:12" ht="30" x14ac:dyDescent="0.25">
       <c r="C67" s="7"/>
       <c r="D67" s="2" t="s">
         <v>48</v>
@@ -1834,8 +1994,14 @@
       <c r="J67">
         <v>5</v>
       </c>
-    </row>
-    <row r="68" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="K67" s="15">
+        <v>0</v>
+      </c>
+      <c r="L67" s="19" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="68" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C68" s="3"/>
       <c r="D68" s="2" t="s">
         <v>90</v>
@@ -1854,7 +2020,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="69" spans="3:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="3:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C69" s="3"/>
       <c r="D69" s="12"/>
       <c r="E69" s="3"/>
@@ -1863,12 +2029,12 @@
       <c r="H69" s="5"/>
       <c r="I69" s="2"/>
     </row>
-    <row r="70" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C70" s="3"/>
       <c r="E70" s="3"/>
       <c r="H70" s="6"/>
     </row>
-    <row r="71" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="3:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C71" s="3"/>
       <c r="D71" s="2"/>
       <c r="E71" s="3"/>
@@ -1877,7 +2043,7 @@
       <c r="H71" s="5"/>
       <c r="I71" s="2"/>
     </row>
-    <row r="72" spans="3:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="3:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C72" s="3"/>
       <c r="D72" s="12" t="s">
         <v>81</v>
@@ -1888,7 +2054,7 @@
       <c r="H72" s="5"/>
       <c r="I72" s="2"/>
     </row>
-    <row r="73" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C73" s="3"/>
       <c r="D73" s="2" t="s">
         <v>82</v>
@@ -1906,8 +2072,14 @@
       <c r="I73" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="74" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K73" s="15">
+        <v>0</v>
+      </c>
+      <c r="L73" s="19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="74" spans="3:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C74" s="3"/>
       <c r="D74" s="2"/>
       <c r="E74" s="3"/>
@@ -1916,7 +2088,7 @@
       <c r="H74" s="5"/>
       <c r="I74" s="2"/>
     </row>
-    <row r="75" spans="3:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="3:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C75" s="3"/>
       <c r="D75" s="12" t="s">
         <v>52</v>
@@ -1927,7 +2099,7 @@
       <c r="H75" s="5"/>
       <c r="I75" s="2"/>
     </row>
-    <row r="76" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C76" s="7"/>
       <c r="D76" s="2" t="s">
         <v>79</v>
@@ -1945,8 +2117,11 @@
       <c r="I76" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="77" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="K76" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C77" s="7"/>
       <c r="D77" s="2" t="s">
         <v>80</v>
@@ -1964,31 +2139,58 @@
       <c r="I77" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="78" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="K77" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C78" s="3"/>
-      <c r="D78" s="2"/>
+      <c r="D78" s="2" t="s">
+        <v>97</v>
+      </c>
       <c r="E78" s="3"/>
-      <c r="F78" s="2"/>
-      <c r="G78" s="2"/>
-      <c r="H78" s="5"/>
-      <c r="I78" s="2"/>
-    </row>
-    <row r="79" spans="3:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F78" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G78" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H78" s="5">
+        <v>30</v>
+      </c>
+      <c r="I78" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K78" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C79" s="3"/>
-      <c r="D79" s="12" t="s">
-        <v>53</v>
+      <c r="D79" s="2" t="s">
+        <v>98</v>
       </c>
       <c r="E79" s="3"/>
-      <c r="F79" s="2"/>
-      <c r="G79" s="2"/>
-      <c r="H79" s="5"/>
-      <c r="I79" s="2"/>
-    </row>
-    <row r="80" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C80" s="7"/>
+      <c r="F79" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G79" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H79" s="5">
+        <v>30</v>
+      </c>
+      <c r="I79" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K79" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C80" s="3"/>
       <c r="D80" s="2" t="s">
-        <v>65</v>
+        <v>99</v>
       </c>
       <c r="E80" s="3"/>
       <c r="F80" s="2" t="s">
@@ -1998,139 +2200,76 @@
         <v>9</v>
       </c>
       <c r="H80" s="5">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="I80" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J80" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="81" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C81" s="7"/>
-      <c r="D81" s="2" t="s">
-        <v>66</v>
-      </c>
+      <c r="K80" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C81" s="3"/>
+      <c r="D81" s="2"/>
       <c r="E81" s="3"/>
-      <c r="F81" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G81" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H81" s="5">
-        <v>20</v>
-      </c>
-      <c r="I81" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J81" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="82" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C82" s="7"/>
-      <c r="D82" s="2" t="s">
-        <v>67</v>
-      </c>
+      <c r="F81" s="2"/>
+      <c r="G81" s="2"/>
+      <c r="H81" s="5"/>
+      <c r="I81" s="2"/>
+    </row>
+    <row r="82" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C82" s="3"/>
+      <c r="D82" s="2"/>
       <c r="E82" s="3"/>
-      <c r="F82" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G82" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H82" s="5">
-        <v>25</v>
-      </c>
-      <c r="I82" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J82" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="83" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C83" s="7"/>
-      <c r="D83" s="2" t="s">
-        <v>68</v>
-      </c>
+      <c r="F82" s="2"/>
+      <c r="G82" s="2"/>
+      <c r="H82" s="5"/>
+      <c r="I82" s="2"/>
+    </row>
+    <row r="83" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C83" s="3"/>
+      <c r="D83" s="2"/>
       <c r="E83" s="3"/>
-      <c r="F83" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G83" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H83" s="5">
-        <v>45</v>
-      </c>
-      <c r="I83" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J83" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="84" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C84" s="7"/>
-      <c r="D84" s="2" t="s">
-        <v>69</v>
-      </c>
+      <c r="F83" s="2"/>
+      <c r="G83" s="2"/>
+      <c r="H83" s="5"/>
+      <c r="I83" s="2"/>
+    </row>
+    <row r="84" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C84" s="3"/>
+      <c r="D84" s="2"/>
       <c r="E84" s="3"/>
-      <c r="F84" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G84" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H84" s="5">
-        <v>25</v>
-      </c>
-      <c r="I84" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J84" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="85" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C85" s="7"/>
-      <c r="D85" s="2" t="s">
-        <v>43</v>
+      <c r="F84" s="2"/>
+      <c r="G84" s="2"/>
+      <c r="H84" s="5"/>
+      <c r="I84" s="2"/>
+    </row>
+    <row r="85" spans="3:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C85" s="3"/>
+      <c r="D85" s="12" t="s">
+        <v>53</v>
       </c>
       <c r="E85" s="3"/>
-      <c r="F85" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G85" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H85" s="5">
-        <v>25</v>
-      </c>
-      <c r="I85" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J85" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="86" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="F85" s="2"/>
+      <c r="G85" s="2"/>
+      <c r="H85" s="5"/>
+      <c r="I85" s="2"/>
+    </row>
+    <row r="86" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C86" s="7"/>
       <c r="D86" s="2" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="E86" s="3"/>
       <c r="F86" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G86" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H86" s="5">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="I86" s="2" t="s">
         <v>15</v>
@@ -2138,33 +2277,67 @@
       <c r="J86" s="9">
         <v>1</v>
       </c>
-    </row>
-    <row r="87" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C87" s="3"/>
-      <c r="D87" s="2"/>
+      <c r="K86" s="15">
+        <v>0</v>
+      </c>
+      <c r="L86" s="19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="87" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C87" s="7"/>
+      <c r="D87" s="2" t="s">
+        <v>66</v>
+      </c>
       <c r="E87" s="3"/>
-      <c r="F87" s="2"/>
-      <c r="G87" s="2"/>
-      <c r="H87" s="5"/>
-      <c r="I87" s="2"/>
-      <c r="J87" s="9"/>
-    </row>
-    <row r="88" spans="3:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C88" s="3"/>
-      <c r="D88" s="12" t="s">
-        <v>54</v>
+      <c r="F87" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G87" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H87" s="5">
+        <v>20</v>
+      </c>
+      <c r="I87" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J87" s="9">
+        <v>1</v>
+      </c>
+      <c r="K87" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C88" s="7"/>
+      <c r="D88" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="E88" s="3"/>
-      <c r="F88" s="2"/>
-      <c r="G88" s="2"/>
-      <c r="H88" s="5"/>
-      <c r="I88" s="2"/>
-      <c r="J88" s="9"/>
-    </row>
-    <row r="89" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F88" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G88" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H88" s="5">
+        <v>25</v>
+      </c>
+      <c r="I88" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J88" s="9">
+        <v>1</v>
+      </c>
+      <c r="K88" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="3:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C89" s="7"/>
       <c r="D89" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E89" s="3"/>
       <c r="F89" s="2" t="s">
@@ -2174,105 +2347,128 @@
         <v>9</v>
       </c>
       <c r="H89" s="5">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="I89" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J89">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="90" spans="3:10" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="J89" s="9">
+        <v>1</v>
+      </c>
+      <c r="K89" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C90" s="7"/>
       <c r="D90" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E90" s="3"/>
       <c r="F90" s="2" t="s">
         <v>18</v>
       </c>
       <c r="G90" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H90" s="5">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="I90" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J90">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="91" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="J90" s="9">
+        <v>1</v>
+      </c>
+      <c r="K90" s="15">
+        <v>0</v>
+      </c>
+      <c r="L90" s="19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="91" spans="3:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C91" s="7"/>
       <c r="D91" s="2" t="s">
-        <v>72</v>
+        <v>43</v>
       </c>
       <c r="E91" s="3"/>
       <c r="F91" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G91" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H91" s="5">
         <v>25</v>
       </c>
       <c r="I91" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J91">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="92" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C92" s="3"/>
-      <c r="D92" s="2"/>
+        <v>15</v>
+      </c>
+      <c r="J91" s="9">
+        <v>1</v>
+      </c>
+      <c r="K91" s="15">
+        <v>0</v>
+      </c>
+      <c r="L91" s="19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="92" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C92" s="7"/>
+      <c r="D92" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="E92" s="3"/>
-      <c r="F92" s="2"/>
-      <c r="G92" s="2"/>
-      <c r="H92" s="5"/>
-      <c r="I92" s="2"/>
-    </row>
-    <row r="93" spans="3:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F92" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G92" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H92" s="5">
+        <v>10</v>
+      </c>
+      <c r="I92" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J92" s="9">
+        <v>1</v>
+      </c>
+      <c r="K92" s="15">
+        <v>0</v>
+      </c>
+      <c r="L92" s="19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="93" spans="3:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C93" s="3"/>
-      <c r="D93" s="12" t="s">
-        <v>55</v>
-      </c>
+      <c r="D93" s="2"/>
       <c r="E93" s="3"/>
       <c r="F93" s="2"/>
       <c r="G93" s="2"/>
       <c r="H93" s="5"/>
       <c r="I93" s="2"/>
-    </row>
-    <row r="94" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C94" s="7"/>
-      <c r="D94" s="2" t="s">
-        <v>73</v>
+      <c r="J93" s="9"/>
+    </row>
+    <row r="94" spans="3:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C94" s="3"/>
+      <c r="D94" s="12" t="s">
+        <v>54</v>
       </c>
       <c r="E94" s="3"/>
-      <c r="F94" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G94" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H94" s="5">
-        <v>30</v>
-      </c>
-      <c r="I94" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J94">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="95" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F94" s="2"/>
+      <c r="G94" s="2"/>
+      <c r="H94" s="5"/>
+      <c r="I94" s="2"/>
+      <c r="J94" s="9"/>
+    </row>
+    <row r="95" spans="3:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C95" s="7"/>
       <c r="D95" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E95" s="3"/>
       <c r="F95" s="2" t="s">
@@ -2282,7 +2478,7 @@
         <v>9</v>
       </c>
       <c r="H95" s="5">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="I95" s="2" t="s">
         <v>16</v>
@@ -2291,20 +2487,20 @@
         <v>5</v>
       </c>
     </row>
-    <row r="96" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C96" s="7"/>
       <c r="D96" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E96" s="3"/>
       <c r="F96" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G96" s="2" t="s">
         <v>9</v>
       </c>
       <c r="H96" s="5">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="I96" s="2" t="s">
         <v>16</v>
@@ -2316,17 +2512,17 @@
     <row r="97" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C97" s="7"/>
       <c r="D97" s="2" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E97" s="3"/>
       <c r="F97" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G97" s="2" t="s">
         <v>9</v>
       </c>
       <c r="H97" s="5">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="I97" s="2" t="s">
         <v>16</v>
@@ -2336,114 +2532,204 @@
       </c>
     </row>
     <row r="98" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C98" s="7"/>
-      <c r="D98" s="2" t="s">
-        <v>77</v>
-      </c>
+      <c r="C98" s="3"/>
+      <c r="D98" s="2"/>
       <c r="E98" s="3"/>
-      <c r="F98" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G98" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H98" s="5">
-        <v>120</v>
-      </c>
-      <c r="I98" s="2" t="s">
+      <c r="F98" s="2"/>
+      <c r="G98" s="2"/>
+      <c r="H98" s="5"/>
+      <c r="I98" s="2"/>
+    </row>
+    <row r="99" spans="3:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C99" s="3"/>
+      <c r="D99" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="E99" s="3"/>
+      <c r="F99" s="2"/>
+      <c r="G99" s="2"/>
+      <c r="H99" s="5"/>
+      <c r="I99" s="2"/>
+    </row>
+    <row r="100" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C100" s="7"/>
+      <c r="D100" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E100" s="3"/>
+      <c r="F100" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G100" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H100" s="5">
+        <v>30</v>
+      </c>
+      <c r="I100" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J98">
+      <c r="J100">
         <v>5</v>
       </c>
     </row>
-    <row r="99" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C99" s="7"/>
-      <c r="D99" t="s">
-        <v>78</v>
-      </c>
-      <c r="F99" t="s">
-        <v>17</v>
-      </c>
-      <c r="G99" t="s">
-        <v>9</v>
-      </c>
-      <c r="H99" s="6">
-        <v>60</v>
-      </c>
-      <c r="I99" t="s">
+    <row r="101" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C101" s="7"/>
+      <c r="D101" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E101" s="3"/>
+      <c r="F101" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G101" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H101" s="5">
+        <v>35</v>
+      </c>
+      <c r="I101" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="100" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C100" s="3"/>
-      <c r="H100" s="6"/>
-    </row>
-    <row r="101" spans="3:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C101" s="3"/>
-      <c r="D101" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="E101" s="3"/>
-      <c r="F101" s="2"/>
-      <c r="G101" s="2"/>
-      <c r="H101" s="5"/>
-      <c r="I101" s="2"/>
+      <c r="J101">
+        <v>5</v>
+      </c>
     </row>
     <row r="102" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C102" s="7"/>
       <c r="D102" s="2" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="E102" s="3"/>
       <c r="F102" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G102" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H102" s="5">
-        <v>180</v>
+        <v>60</v>
       </c>
       <c r="I102" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="J102">
+        <v>5</v>
+      </c>
     </row>
     <row r="103" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C103" s="7"/>
-      <c r="D103" t="s">
+      <c r="D103" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E103" s="3"/>
+      <c r="F103" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G103" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H103" s="5">
+        <v>35</v>
+      </c>
+      <c r="I103" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J103">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="104" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C104" s="7"/>
+      <c r="D104" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E104" s="3"/>
+      <c r="F104" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G104" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H104" s="5">
+        <v>120</v>
+      </c>
+      <c r="I104" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J104">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="105" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C105" s="7"/>
+      <c r="D105" t="s">
+        <v>78</v>
+      </c>
+      <c r="F105" t="s">
+        <v>17</v>
+      </c>
+      <c r="G105" t="s">
+        <v>9</v>
+      </c>
+      <c r="H105" s="6">
+        <v>60</v>
+      </c>
+      <c r="I105" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="106" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C106" s="3"/>
+      <c r="H106" s="6"/>
+    </row>
+    <row r="107" spans="3:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C107" s="3"/>
+      <c r="D107" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="E107" s="3"/>
+      <c r="F107" s="2"/>
+      <c r="G107" s="2"/>
+      <c r="H107" s="5"/>
+      <c r="I107" s="2"/>
+    </row>
+    <row r="108" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C108" s="7"/>
+      <c r="D108" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E108" s="3"/>
+      <c r="F108" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G108" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H108" s="5">
+        <v>180</v>
+      </c>
+      <c r="I108" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="109" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C109" s="7"/>
+      <c r="D109" t="s">
         <v>47</v>
       </c>
-      <c r="F103" t="s">
+      <c r="F109" t="s">
         <v>18</v>
       </c>
-      <c r="G103" t="s">
+      <c r="G109" t="s">
         <v>8</v>
       </c>
-      <c r="H103" s="6">
+      <c r="H109" s="6">
         <v>30</v>
       </c>
-      <c r="I103" t="s">
+      <c r="I109" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="104" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="H104" s="6"/>
-    </row>
-    <row r="105" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="H105" s="6"/>
-    </row>
-    <row r="106" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="H106" s="6"/>
-    </row>
-    <row r="107" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="H107" s="6"/>
-    </row>
-    <row r="108" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="H108" s="6"/>
-    </row>
-    <row r="109" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="H109" s="6"/>
     </row>
     <row r="110" spans="3:10" x14ac:dyDescent="0.25">
       <c r="H110" s="6"/>
@@ -2540,6 +2826,24 @@
     </row>
     <row r="141" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H141" s="6"/>
+    </row>
+    <row r="142" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H142" s="6"/>
+    </row>
+    <row r="143" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H143" s="6"/>
+    </row>
+    <row r="144" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H144" s="6"/>
+    </row>
+    <row r="145" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H145" s="6"/>
+    </row>
+    <row r="146" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H146" s="6"/>
+    </row>
+    <row r="147" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H147" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2547,13 +2851,13 @@
     <mergeCell ref="C4:D4"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G15:G21 G23:G42 G71:G188 G44:G69" xr:uid="{737FDF90-EFB8-4011-8F39-3F216A04A4E8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G15:G21 G23:G42 G71:G194 G44:G69" xr:uid="{737FDF90-EFB8-4011-8F39-3F216A04A4E8}">
       <formula1>$G$4:$G$7</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I13:I21 I23:I42 I71:I141 I44:I69" xr:uid="{D545C4CF-8505-4E3A-8974-2AE18E2A1E4D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I13:I21 I23:I42 I71:I147 I44:I69" xr:uid="{D545C4CF-8505-4E3A-8974-2AE18E2A1E4D}">
       <formula1>$H$4:$H$6</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F13:F21 F23:F42 F71:F141 F44:F69" xr:uid="{0789BEBC-1BFC-4915-ADA0-26973175C7BB}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F13:F21 F23:F42 F71:F147 F44:F69" xr:uid="{0789BEBC-1BFC-4915-ADA0-26973175C7BB}">
       <formula1>$F$4:$F$6</formula1>
     </dataValidation>
   </dataValidations>
@@ -2600,15 +2904,15 @@
         <v>14</v>
       </c>
       <c r="E7" s="8">
-        <f>COUNTIF(Plannification!I13:I141,Plannification!H4)</f>
+        <f>COUNTIF(Plannification!I13:I147,Plannification!H4)</f>
         <v>24</v>
       </c>
       <c r="F7" s="11">
-        <f>(COUNTIFS(Plannification!G:G,"Facile",Plannification!I:I,"Sprint 1")*1+COUNTIFS(Plannification!G:G,"Moyen",Plannification!I:I,"Sprint 1")*5+COUNTIFS(Plannification!G:G,"Difficile",Plannification!I:I,"Sprint 1")*10+COUNTIFS(Plannification!G:G,"Incertain",Plannification!I:I,"Sprint 1")*7.5)/COUNTA(Plannification!G13:G102)</f>
-        <v>1.7946428571428572</v>
+        <f>(COUNTIFS(Plannification!G:G,"Facile",Plannification!I:I,"Sprint 1")*1+COUNTIFS(Plannification!G:G,"Moyen",Plannification!I:I,"Sprint 1")*5+COUNTIFS(Plannification!G:G,"Difficile",Plannification!I:I,"Sprint 1")*10+COUNTIFS(Plannification!G:G,"Incertain",Plannification!I:I,"Sprint 1")*7.5)/COUNTA(Plannification!G13:G108)</f>
+        <v>1.7033898305084745</v>
       </c>
       <c r="G7">
-        <f>SUMIF(Plannification!I13:I140,Plannification!H4,Plannification!H13:H140)</f>
+        <f>SUMIF(Plannification!I13:I146,Plannification!H4,Plannification!H13:H146)</f>
         <v>1260</v>
       </c>
     </row>
@@ -2617,16 +2921,16 @@
         <v>15</v>
       </c>
       <c r="E8">
-        <f>COUNTIF(Plannification!I13:I141,Plannification!H5)</f>
-        <v>19</v>
+        <f>COUNTIF(Plannification!I13:I147,Plannification!H5)</f>
+        <v>22</v>
       </c>
       <c r="F8" s="11">
-        <f>(COUNTIFS(Plannification!G:G,"Facile",Plannification!I:I,"Sprint 2")*1+COUNTIFS(Plannification!G:G,"Moyen",Plannification!I:I,"Sprint 2")*5+COUNTIFS(Plannification!G:G,"Difficile",Plannification!I:I,"Sprint 2")*10+COUNTIFS(Plannification!G:G,"Incertain",Plannification!I:I,"Sprint 2")*7.5)/COUNTA(Plannification!G13:G102)</f>
-        <v>1.5178571428571428</v>
+        <f>(COUNTIFS(Plannification!G:G,"Facile",Plannification!I:I,"Sprint 2")*1+COUNTIFS(Plannification!G:G,"Moyen",Plannification!I:I,"Sprint 2")*5+COUNTIFS(Plannification!G:G,"Difficile",Plannification!I:I,"Sprint 2")*10+COUNTIFS(Plannification!G:G,"Incertain",Plannification!I:I,"Sprint 2")*7.5)/COUNTA(Plannification!G13:G108)</f>
+        <v>1.5593220338983051</v>
       </c>
       <c r="G8">
-        <f>SUMIF(Plannification!I13:I140,Plannification!H5,Plannification!H13:H140)</f>
-        <v>1095</v>
+        <f>SUMIF(Plannification!I13:I146,Plannification!H5,Plannification!H13:H146)</f>
+        <v>1215</v>
       </c>
     </row>
     <row r="9" spans="4:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2634,15 +2938,15 @@
         <v>16</v>
       </c>
       <c r="E9">
-        <f>COUNTIF(Plannification!I13:I141,Plannification!H6)</f>
+        <f>COUNTIF(Plannification!I13:I147,Plannification!H6)</f>
         <v>14</v>
       </c>
       <c r="F9" s="11">
-        <f>(COUNTIFS(Plannification!G:G,"Facile",Plannification!I:I,"Sprint 3")*1+COUNTIFS(Plannification!G:G,"Moyen",Plannification!I:I,"Sprint 3")*5+COUNTIFS(Plannification!G:G,"Difficile",Plannification!I:I,"Sprint 3")*10+COUNTIFS(Plannification!G:G,"Incertain",Plannification!I:I,"Sprint 3")*7.5)/COUNTA(Plannification!G13:G102)</f>
-        <v>1.2410714285714286</v>
+        <f>(COUNTIFS(Plannification!G:G,"Facile",Plannification!I:I,"Sprint 3")*1+COUNTIFS(Plannification!G:G,"Moyen",Plannification!I:I,"Sprint 3")*5+COUNTIFS(Plannification!G:G,"Difficile",Plannification!I:I,"Sprint 3")*10+COUNTIFS(Plannification!G:G,"Incertain",Plannification!I:I,"Sprint 3")*7.5)/COUNTA(Plannification!G13:G108)</f>
+        <v>1.1779661016949152</v>
       </c>
       <c r="G9">
-        <f>SUMIF(Plannification!I13:I140,Plannification!H6,Plannification!H13:H140)</f>
+        <f>SUMIF(Plannification!I13:I146,Plannification!H6,Plannification!H13:H146)</f>
         <v>840</v>
       </c>
     </row>
@@ -2655,15 +2959,15 @@
       </c>
       <c r="E11">
         <f>SUM(E7:E10)</f>
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="F11" s="11">
         <f>AVERAGE(F7:F9)</f>
-        <v>1.517857142857143</v>
+        <v>1.4802259887005649</v>
       </c>
       <c r="G11" s="11">
         <f>(G7+G8+G9)</f>
-        <v>3195</v>
+        <v>3315</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added keyboard html, css and js in normal game
</commit_message>
<xml_diff>
--- a/C61/Phase 1/Plannification.xlsx
+++ b/C61/Phase 1/Plannification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\CEGEP\Shift\C61\Phase 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBBE38D8-9BDF-4538-B408-FC3C84885C8A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBA19987-07E0-4E44-BDFB-300D4FCDD4DD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{BF791A61-1AC1-4C7E-B497-ABC8E6F84FF9}"/>
   </bookViews>
@@ -447,8 +447,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -466,19 +464,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="8">
     <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
       <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -534,8 +534,8 @@
     <tableColumn id="9" xr3:uid="{4BB0A79B-2A72-4D99-BAAE-1417C9CAB8ED}" name="Estimation du temps (Minutes)" dataDxfId="3"/>
     <tableColumn id="10" xr3:uid="{1E1E24DC-14B2-493C-89A6-C8A50BD4426E}" name="No Sprint"/>
     <tableColumn id="2" xr3:uid="{A39DC1DB-5846-4641-8706-F0F11BD2DE3F}" name="Colonne1"/>
-    <tableColumn id="3" xr3:uid="{C66CE7BF-5C52-44E8-8EF8-E28096D37B9A}" name="%" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{70C6D8C4-FE57-4C67-9C5A-4753AD78373B}" name="Explication" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{C66CE7BF-5C52-44E8-8EF8-E28096D37B9A}" name="%" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{70C6D8C4-FE57-4C67-9C5A-4753AD78373B}" name="Explication" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -547,7 +547,7 @@
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{7129546F-9161-4E67-83CD-24985F439177}" name="Sprint"/>
     <tableColumn id="3" xr3:uid="{EE02ED3A-9EB9-4163-82D8-E449A890A7D2}" name="Nombre de tâche"/>
-    <tableColumn id="4" xr3:uid="{7A15D220-8097-4D1D-9F42-CA005B326E2A}" name="Difficulté moyenne" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{7A15D220-8097-4D1D-9F42-CA005B326E2A}" name="Difficulté moyenne" dataDxfId="0"/>
     <tableColumn id="5" xr3:uid="{20438E1E-C106-4680-8557-D00CA50BC5A6}" name="Temps total requis"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -853,8 +853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33D8B194-C08B-45A7-8AEE-FF27905754D6}">
   <dimension ref="C3:L147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="K56" sqref="K56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -867,8 +867,8 @@
     <col min="8" max="8" width="14.7109375" customWidth="1"/>
     <col min="9" max="9" width="14.85546875" customWidth="1"/>
     <col min="10" max="10" width="0" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="11.140625" style="15" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="37.85546875" style="19" customWidth="1"/>
+    <col min="11" max="11" width="11.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="37.85546875" style="17" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:12" x14ac:dyDescent="0.25">
@@ -877,10 +877,10 @@
       </c>
     </row>
     <row r="4" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="14"/>
+      <c r="D4" s="21"/>
       <c r="F4" s="10" t="s">
         <v>17</v>
       </c>
@@ -917,10 +917,10 @@
       </c>
     </row>
     <row r="7" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="14"/>
+      <c r="D7" s="21"/>
       <c r="F7" s="10"/>
       <c r="G7" s="10" t="s">
         <v>11</v>
@@ -952,10 +952,10 @@
       <c r="J12" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="K12" s="16" t="s">
+      <c r="K12" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="L12" s="20" t="s">
+      <c r="L12" s="18" t="s">
         <v>92</v>
       </c>
     </row>
@@ -980,10 +980,10 @@
       <c r="J13" s="9">
         <v>1</v>
       </c>
-      <c r="K13" s="17">
-        <v>1</v>
-      </c>
-      <c r="L13" s="21"/>
+      <c r="K13" s="15">
+        <v>1</v>
+      </c>
+      <c r="L13" s="19"/>
     </row>
     <row r="14" spans="3:12" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="7"/>
@@ -1006,10 +1006,10 @@
       <c r="J14" s="9">
         <v>1</v>
       </c>
-      <c r="K14" s="17">
+      <c r="K14" s="15">
         <v>0.75</v>
       </c>
-      <c r="L14" s="21" t="s">
+      <c r="L14" s="19" t="s">
         <v>101</v>
       </c>
     </row>
@@ -1034,7 +1034,7 @@
       <c r="J15" s="9">
         <v>1</v>
       </c>
-      <c r="K15" s="18">
+      <c r="K15" s="16">
         <v>1</v>
       </c>
     </row>
@@ -1081,7 +1081,7 @@
       <c r="J18">
         <v>5</v>
       </c>
-      <c r="K18" s="18">
+      <c r="K18" s="16">
         <v>1</v>
       </c>
     </row>
@@ -1106,10 +1106,10 @@
       <c r="J19" s="9">
         <v>1</v>
       </c>
-      <c r="K19" s="18">
+      <c r="K19" s="16">
         <v>0.33</v>
       </c>
-      <c r="L19" s="19" t="s">
+      <c r="L19" s="17" t="s">
         <v>93</v>
       </c>
     </row>
@@ -1163,7 +1163,7 @@
       <c r="J23">
         <v>5</v>
       </c>
-      <c r="K23" s="15">
+      <c r="K23" s="13">
         <v>1</v>
       </c>
     </row>
@@ -1188,7 +1188,7 @@
       <c r="J24">
         <v>5</v>
       </c>
-      <c r="K24" s="15">
+      <c r="K24" s="13">
         <v>1</v>
       </c>
     </row>
@@ -1232,7 +1232,7 @@
       <c r="I26" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="K26" s="15">
+      <c r="K26" s="13">
         <v>1</v>
       </c>
     </row>
@@ -1254,7 +1254,7 @@
       <c r="I27" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K27" s="15">
+      <c r="K27" s="13">
         <v>1</v>
       </c>
     </row>
@@ -1276,7 +1276,7 @@
       <c r="I28" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K28" s="15">
+      <c r="K28" s="13">
         <v>1</v>
       </c>
     </row>
@@ -1298,7 +1298,7 @@
       <c r="I29" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K29" s="15">
+      <c r="K29" s="13">
         <v>1</v>
       </c>
     </row>
@@ -1367,10 +1367,10 @@
       <c r="I35" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="K35" s="15">
+      <c r="K35" s="13">
         <v>0.85</v>
       </c>
-      <c r="L35" s="19" t="s">
+      <c r="L35" s="17" t="s">
         <v>100</v>
       </c>
     </row>
@@ -1392,10 +1392,10 @@
       <c r="I36" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="K36" s="15">
+      <c r="K36" s="13">
         <v>0.85</v>
       </c>
-      <c r="L36" s="19" t="s">
+      <c r="L36" s="17" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1439,7 +1439,7 @@
       <c r="J38">
         <v>5</v>
       </c>
-      <c r="K38" s="15">
+      <c r="K38" s="13">
         <v>1</v>
       </c>
     </row>
@@ -1480,7 +1480,7 @@
       <c r="I40" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K40" s="15">
+      <c r="K40" s="13">
         <v>1</v>
       </c>
     </row>
@@ -1541,7 +1541,7 @@
       <c r="J45" s="9">
         <v>1</v>
       </c>
-      <c r="K45" s="18">
+      <c r="K45" s="16">
         <v>1</v>
       </c>
     </row>
@@ -1566,7 +1566,7 @@
       <c r="J46" s="9">
         <v>1</v>
       </c>
-      <c r="K46" s="18">
+      <c r="K46" s="16">
         <v>1</v>
       </c>
     </row>
@@ -1591,7 +1591,7 @@
       <c r="J47" s="9">
         <v>1</v>
       </c>
-      <c r="K47" s="18">
+      <c r="K47" s="16">
         <v>1</v>
       </c>
     </row>
@@ -1614,7 +1614,7 @@
         <v>14</v>
       </c>
       <c r="J48" s="9"/>
-      <c r="K48" s="18">
+      <c r="K48" s="16">
         <v>1</v>
       </c>
     </row>
@@ -1639,7 +1639,7 @@
       <c r="J49">
         <v>5</v>
       </c>
-      <c r="K49" s="18">
+      <c r="K49" s="16">
         <v>1</v>
       </c>
     </row>
@@ -1703,7 +1703,7 @@
       <c r="J53">
         <v>5</v>
       </c>
-      <c r="K53" s="15">
+      <c r="K53" s="13">
         <v>0</v>
       </c>
     </row>
@@ -1728,7 +1728,7 @@
       <c r="J54">
         <v>5</v>
       </c>
-      <c r="K54" s="15">
+      <c r="K54" s="13">
         <v>0</v>
       </c>
     </row>
@@ -1753,6 +1753,9 @@
       <c r="J55" s="9">
         <v>1</v>
       </c>
+      <c r="K55" s="13">
+        <v>1</v>
+      </c>
     </row>
     <row r="56" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C56" s="7"/>
@@ -1797,7 +1800,7 @@
       <c r="J57">
         <v>5</v>
       </c>
-      <c r="K57" s="18"/>
+      <c r="K57" s="16"/>
     </row>
     <row r="58" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C58" s="3"/>
@@ -1840,7 +1843,7 @@
       <c r="J60" s="9">
         <v>1</v>
       </c>
-      <c r="K60" s="15">
+      <c r="K60" s="13">
         <v>1</v>
       </c>
     </row>
@@ -1865,10 +1868,10 @@
       <c r="J61">
         <v>5</v>
       </c>
-      <c r="K61" s="15">
+      <c r="K61" s="13">
         <v>0</v>
       </c>
-      <c r="L61" s="19" t="s">
+      <c r="L61" s="17" t="s">
         <v>95</v>
       </c>
     </row>
@@ -1893,10 +1896,10 @@
       <c r="J62">
         <v>5</v>
       </c>
-      <c r="K62" s="15">
+      <c r="K62" s="13">
         <v>0</v>
       </c>
-      <c r="L62" s="19" t="s">
+      <c r="L62" s="17" t="s">
         <v>95</v>
       </c>
     </row>
@@ -1941,7 +1944,7 @@
       <c r="J65">
         <v>7.5</v>
       </c>
-      <c r="K65" s="15">
+      <c r="K65" s="13">
         <v>1</v>
       </c>
     </row>
@@ -1966,10 +1969,10 @@
       <c r="J66">
         <v>5</v>
       </c>
-      <c r="K66" s="15">
+      <c r="K66" s="13">
         <v>0</v>
       </c>
-      <c r="L66" s="19" t="s">
+      <c r="L66" s="17" t="s">
         <v>95</v>
       </c>
     </row>
@@ -1994,10 +1997,10 @@
       <c r="J67">
         <v>5</v>
       </c>
-      <c r="K67" s="15">
+      <c r="K67" s="13">
         <v>0</v>
       </c>
-      <c r="L67" s="19" t="s">
+      <c r="L67" s="17" t="s">
         <v>95</v>
       </c>
     </row>
@@ -2072,10 +2075,10 @@
       <c r="I73" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K73" s="15">
+      <c r="K73" s="13">
         <v>0</v>
       </c>
-      <c r="L73" s="19" t="s">
+      <c r="L73" s="17" t="s">
         <v>96</v>
       </c>
     </row>
@@ -2117,7 +2120,7 @@
       <c r="I76" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K76" s="15">
+      <c r="K76" s="13">
         <v>1</v>
       </c>
     </row>
@@ -2139,7 +2142,7 @@
       <c r="I77" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K77" s="15">
+      <c r="K77" s="13">
         <v>1</v>
       </c>
     </row>
@@ -2161,7 +2164,7 @@
       <c r="I78" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K78" s="15">
+      <c r="K78" s="13">
         <v>1</v>
       </c>
     </row>
@@ -2183,7 +2186,7 @@
       <c r="I79" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K79" s="15">
+      <c r="K79" s="13">
         <v>1</v>
       </c>
     </row>
@@ -2205,7 +2208,7 @@
       <c r="I80" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K80" s="15">
+      <c r="K80" s="13">
         <v>1</v>
       </c>
     </row>
@@ -2277,10 +2280,10 @@
       <c r="J86" s="9">
         <v>1</v>
       </c>
-      <c r="K86" s="15">
+      <c r="K86" s="13">
         <v>0</v>
       </c>
-      <c r="L86" s="19" t="s">
+      <c r="L86" s="17" t="s">
         <v>96</v>
       </c>
     </row>
@@ -2305,7 +2308,7 @@
       <c r="J87" s="9">
         <v>1</v>
       </c>
-      <c r="K87" s="15">
+      <c r="K87" s="13">
         <v>1</v>
       </c>
     </row>
@@ -2330,7 +2333,7 @@
       <c r="J88" s="9">
         <v>1</v>
       </c>
-      <c r="K88" s="15">
+      <c r="K88" s="13">
         <v>1</v>
       </c>
     </row>
@@ -2355,7 +2358,7 @@
       <c r="J89" s="9">
         <v>1</v>
       </c>
-      <c r="K89" s="15">
+      <c r="K89" s="13">
         <v>1</v>
       </c>
     </row>
@@ -2380,10 +2383,10 @@
       <c r="J90" s="9">
         <v>1</v>
       </c>
-      <c r="K90" s="15">
+      <c r="K90" s="13">
         <v>0</v>
       </c>
-      <c r="L90" s="19" t="s">
+      <c r="L90" s="17" t="s">
         <v>96</v>
       </c>
     </row>
@@ -2408,10 +2411,10 @@
       <c r="J91" s="9">
         <v>1</v>
       </c>
-      <c r="K91" s="15">
+      <c r="K91" s="13">
         <v>0</v>
       </c>
-      <c r="L91" s="19" t="s">
+      <c r="L91" s="17" t="s">
         <v>96</v>
       </c>
     </row>
@@ -2436,10 +2439,10 @@
       <c r="J92" s="9">
         <v>1</v>
       </c>
-      <c r="K92" s="15">
+      <c r="K92" s="13">
         <v>0</v>
       </c>
-      <c r="L92" s="19" t="s">
+      <c r="L92" s="17" t="s">
         <v>96</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added count of each language of game played
</commit_message>
<xml_diff>
--- a/C61/Phase 1/Plannification.xlsx
+++ b/C61/Phase 1/Plannification.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\CEGEP\Shift\C61\Phase 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBA19987-07E0-4E44-BDFB-300D4FCDD4DD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3057F7E-902D-432C-B546-CE5B980B6D17}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{BF791A61-1AC1-4C7E-B497-ABC8E6F84FF9}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="102">
   <si>
     <t>Nom</t>
   </si>
@@ -853,8 +853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33D8B194-C08B-45A7-8AEE-FF27905754D6}">
   <dimension ref="C3:L147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="K56" sqref="K56"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1192,7 +1192,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:12" ht="30" x14ac:dyDescent="0.25">
       <c r="C25" s="7"/>
       <c r="D25" s="2" t="s">
         <v>25</v>
@@ -1212,6 +1212,12 @@
       </c>
       <c r="J25">
         <v>5</v>
+      </c>
+      <c r="K25" s="13">
+        <v>0</v>
+      </c>
+      <c r="L25" s="17" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="26" spans="3:12" x14ac:dyDescent="0.25">
@@ -1618,7 +1624,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C49" s="7"/>
       <c r="D49" s="2" t="s">
         <v>38</v>
@@ -1643,7 +1649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C50" s="7"/>
       <c r="D50" s="2" t="s">
         <v>45</v>
@@ -1662,7 +1668,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="51" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C51" s="3"/>
       <c r="D51" s="2"/>
       <c r="E51" s="3"/>
@@ -1671,7 +1677,7 @@
       <c r="H51" s="5"/>
       <c r="I51" s="2"/>
     </row>
-    <row r="52" spans="3:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="3:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C52" s="3"/>
       <c r="D52" s="12" t="s">
         <v>58</v>
@@ -1682,7 +1688,7 @@
       <c r="H52" s="5"/>
       <c r="I52" s="2"/>
     </row>
-    <row r="53" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C53" s="7"/>
       <c r="D53" s="2" t="s">
         <v>48</v>
@@ -1707,7 +1713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C54" s="7"/>
       <c r="D54" s="2" t="s">
         <v>62</v>
@@ -1732,7 +1738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C55" s="7"/>
       <c r="D55" s="2" t="s">
         <v>49</v>
@@ -1757,7 +1763,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C56" s="7"/>
       <c r="D56" s="2" t="s">
         <v>50</v>
@@ -1779,7 +1785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C57" s="7"/>
       <c r="D57" s="2" t="s">
         <v>51</v>
@@ -1802,7 +1808,7 @@
       </c>
       <c r="K57" s="16"/>
     </row>
-    <row r="58" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C58" s="3"/>
       <c r="D58" s="2"/>
       <c r="E58" s="3"/>
@@ -1811,7 +1817,7 @@
       <c r="H58" s="5"/>
       <c r="I58" s="2"/>
     </row>
-    <row r="59" spans="3:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="3:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C59" s="3"/>
       <c r="D59" s="12" t="s">
         <v>59</v>
@@ -1822,7 +1828,7 @@
       <c r="H59" s="5"/>
       <c r="I59" s="2"/>
     </row>
-    <row r="60" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C60" s="7"/>
       <c r="D60" s="2" t="s">
         <v>49</v>
@@ -1847,7 +1853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="3:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C61" s="7"/>
       <c r="D61" s="2" t="s">
         <v>62</v>
@@ -1869,13 +1875,10 @@
         <v>5</v>
       </c>
       <c r="K61" s="13">
-        <v>0</v>
-      </c>
-      <c r="L61" s="17" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="62" spans="3:12" ht="30" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C62" s="7"/>
       <c r="D62" s="2" t="s">
         <v>48</v>
@@ -1897,13 +1900,10 @@
         <v>5</v>
       </c>
       <c r="K62" s="13">
-        <v>0</v>
-      </c>
-      <c r="L62" s="17" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="63" spans="3:12" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C63" s="3"/>
       <c r="D63" s="2"/>
       <c r="E63" s="3"/>
@@ -1912,7 +1912,7 @@
       <c r="H63" s="5"/>
       <c r="I63" s="2"/>
     </row>
-    <row r="64" spans="3:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="3:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C64" s="3"/>
       <c r="D64" s="12" t="s">
         <v>63</v>

</xml_diff>

<commit_message>
Added missing features for history page
</commit_message>
<xml_diff>
--- a/C61/Phase 1/Plannification.xlsx
+++ b/C61/Phase 1/Plannification.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\CEGEP\Shift\C61\Phase 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\CEGEP\Shift v2\C61\Phase 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3057F7E-902D-432C-B546-CE5B980B6D17}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F9DF794-153E-46E3-AC02-7FF171EC6BEF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{BF791A61-1AC1-4C7E-B497-ABC8E6F84FF9}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="103">
   <si>
     <t>Nom</t>
   </si>
@@ -336,10 +336,13 @@
     <t>calcPX</t>
   </si>
   <si>
-    <t>Il manque le footer - Le style de cette page a pris beaucoup plus de temps que prévu</t>
-  </si>
-  <si>
-    <t>Manque quelques images</t>
+    <t>Quelques images manquantes</t>
+  </si>
+  <si>
+    <t>J'aimerais prendre un peu de temps pour améliorer l'aspect visuel</t>
+  </si>
+  <si>
+    <t>Pas une priorité. Repoussé au sprint 3 si le temps me le permet - Fonction pour un administrateur</t>
   </si>
 </sst>
 </file>
@@ -853,8 +856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33D8B194-C08B-45A7-8AEE-FF27905754D6}">
   <dimension ref="C3:L147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="L29" sqref="L29"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1010,7 +1013,7 @@
         <v>0.75</v>
       </c>
       <c r="L14" s="19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="3:12" x14ac:dyDescent="0.25">
@@ -1355,7 +1358,7 @@
       <c r="H34" s="5"/>
       <c r="I34" s="2"/>
     </row>
-    <row r="35" spans="3:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C35" s="3"/>
       <c r="D35" s="2" t="s">
         <v>27</v>
@@ -1374,10 +1377,7 @@
         <v>14</v>
       </c>
       <c r="K35" s="13">
-        <v>0.85</v>
-      </c>
-      <c r="L35" s="17" t="s">
-        <v>100</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="3:12" ht="30" x14ac:dyDescent="0.25">
@@ -1424,7 +1424,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:12" ht="30" x14ac:dyDescent="0.25">
       <c r="C38" s="7"/>
       <c r="D38" s="2" t="s">
         <v>30</v>
@@ -1446,7 +1446,10 @@
         <v>5</v>
       </c>
       <c r="K38" s="13">
-        <v>1</v>
+        <v>0.9</v>
+      </c>
+      <c r="L38" s="17" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="39" spans="3:12" x14ac:dyDescent="0.25">
@@ -1624,7 +1627,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C49" s="7"/>
       <c r="D49" s="2" t="s">
         <v>38</v>
@@ -1649,7 +1652,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C50" s="7"/>
       <c r="D50" s="2" t="s">
         <v>45</v>
@@ -1668,7 +1671,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="51" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C51" s="3"/>
       <c r="D51" s="2"/>
       <c r="E51" s="3"/>
@@ -1677,7 +1680,7 @@
       <c r="H51" s="5"/>
       <c r="I51" s="2"/>
     </row>
-    <row r="52" spans="3:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="3:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C52" s="3"/>
       <c r="D52" s="12" t="s">
         <v>58</v>
@@ -1688,7 +1691,7 @@
       <c r="H52" s="5"/>
       <c r="I52" s="2"/>
     </row>
-    <row r="53" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:12" ht="45" x14ac:dyDescent="0.25">
       <c r="C53" s="7"/>
       <c r="D53" s="2" t="s">
         <v>48</v>
@@ -1712,8 +1715,11 @@
       <c r="K53" s="13">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="L53" s="17" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="54" spans="3:12" ht="45" x14ac:dyDescent="0.25">
       <c r="C54" s="7"/>
       <c r="D54" s="2" t="s">
         <v>62</v>
@@ -1737,8 +1743,11 @@
       <c r="K54" s="13">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="L54" s="17" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="55" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C55" s="7"/>
       <c r="D55" s="2" t="s">
         <v>49</v>
@@ -1763,7 +1772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:12" ht="45" x14ac:dyDescent="0.25">
       <c r="C56" s="7"/>
       <c r="D56" s="2" t="s">
         <v>50</v>
@@ -1784,8 +1793,14 @@
       <c r="J56" s="9">
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="K56" s="13">
+        <v>0</v>
+      </c>
+      <c r="L56" s="17" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="57" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C57" s="7"/>
       <c r="D57" s="2" t="s">
         <v>51</v>
@@ -1806,9 +1821,11 @@
       <c r="J57">
         <v>5</v>
       </c>
-      <c r="K57" s="16"/>
-    </row>
-    <row r="58" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="K57" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C58" s="3"/>
       <c r="D58" s="2"/>
       <c r="E58" s="3"/>
@@ -1817,7 +1834,7 @@
       <c r="H58" s="5"/>
       <c r="I58" s="2"/>
     </row>
-    <row r="59" spans="3:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="3:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C59" s="3"/>
       <c r="D59" s="12" t="s">
         <v>59</v>
@@ -1828,7 +1845,7 @@
       <c r="H59" s="5"/>
       <c r="I59" s="2"/>
     </row>
-    <row r="60" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C60" s="7"/>
       <c r="D60" s="2" t="s">
         <v>49</v>
@@ -1853,7 +1870,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C61" s="7"/>
       <c r="D61" s="2" t="s">
         <v>62</v>
@@ -1878,7 +1895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C62" s="7"/>
       <c r="D62" s="2" t="s">
         <v>48</v>
@@ -1903,7 +1920,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C63" s="3"/>
       <c r="D63" s="2"/>
       <c r="E63" s="3"/>
@@ -1912,7 +1929,7 @@
       <c r="H63" s="5"/>
       <c r="I63" s="2"/>
     </row>
-    <row r="64" spans="3:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="3:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C64" s="3"/>
       <c r="D64" s="12" t="s">
         <v>63</v>

</xml_diff>